<commit_message>
Setting "metadata" for reports and inputing first report from SERNAPESCA
</commit_message>
<xml_diff>
--- a/information/reports/summary_reports.xlsx
+++ b/information/reports/summary_reports.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43863C11-50C9-4F15-9F2C-64D0047FEE31}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +19,82 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Name file</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Downloaded date</t>
+  </si>
+  <si>
+    <t>Downloaded from</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Path within reports folder</t>
+  </si>
+  <si>
+    <t>Relevant content</t>
+  </si>
+  <si>
+    <t>indicadores_actividad_pesquera_y_acuicuola_2016_2017.pdf</t>
+  </si>
+  <si>
+    <t>Relevant for scope</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broad overview of the value chain (Figure 1) and self-reporting system in Chile. </t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>SERNAPESCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Periodic report comparing variations of main fishing statistics within each sector relative to previous year </t>
+  </si>
+  <si>
+    <t>Comparng 2017 (January - September) to same period in 2016</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Tittle report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Source </t>
+  </si>
+  <si>
+    <t>Landing data from SERNAPESCA</t>
+  </si>
+  <si>
+    <t>INDICADORES DE ACTIVIDAD PESQUERA EXTRACTIVA Y
+ACUÍCOLA.- Principales Pesquerías Variaciones Mensuales año 2016/2017.
+PERIODO ENERO - SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>Departamento GIA, SERNAPESCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.sernapesca.cl/informes/resultados-gestion </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +102,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +141,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +435,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="12" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3">
+        <v>43327</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{CC9A8E9E-D21F-40B0-9C97-44BCD5770B49}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>